<commit_message>
Fixed wafermap formatting errors
</commit_message>
<xml_diff>
--- a/_G3YR12_G3YR12-24F1.xlsx
+++ b/_G3YR12_G3YR12-24F1.xlsx
@@ -111,13 +111,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF6F9D4"/>
+        <fgColor rgb="FFDEE6EF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDEE6EF"/>
+        <fgColor rgb="FF999999"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>

</xml_diff>